<commit_message>
Actualizado Excel a 2.0
</commit_message>
<xml_diff>
--- a/pruebasProyectoFinal.xlsx
+++ b/pruebasProyectoFinal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brigi\Music\ProyectoFinalMain-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brigi\OneDrive\Escritorio\git_final_proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5064AFD8-F68B-443A-A934-AC0980B7E511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DB8607-00A0-4472-8759-CBF4754A94AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BCD56C2B-7EFC-4439-B006-08DEE2259B23}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>Hacer click a los links (a href)</t>
   </si>
   <si>
-    <t>Proyecto Final Coder House Python (Comisión 27615)</t>
-  </si>
-  <si>
     <t>Francisco Jose Salcedo Morales</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>Lima, Peru</t>
+  </si>
+  <si>
+    <t>Proyecto Final Coder House Python (Comisión 50215)</t>
   </si>
 </sst>
 </file>
@@ -260,10 +260,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,7 +581,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,65 +598,65 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="6"/>
+      <c r="B1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="7"/>
       <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="6"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="6"/>
+      <c r="E2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="6"/>
+      <c r="B3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="7"/>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="6"/>
+      <c r="E3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="6"/>
+      <c r="B4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="7"/>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="6"/>
+      <c r="E4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -746,13 +746,13 @@
         <v>45379</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="E10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>16</v>
@@ -766,13 +766,13 @@
         <v>45379</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>16</v>
@@ -786,13 +786,13 @@
         <v>45379</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="E12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>16</v>
@@ -806,13 +806,13 @@
         <v>45379</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="E13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>16</v>
@@ -826,13 +826,13 @@
         <v>45379</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>16</v>
@@ -849,10 +849,10 @@
         <v>20</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>16</v>
@@ -869,10 +869,10 @@
         <v>21</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>16</v>
@@ -886,13 +886,13 @@
         <v>45379</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>16</v>
@@ -906,18 +906,18 @@
         <v>45379</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="E18" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="7"/>
+      <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
@@ -927,13 +927,13 @@
         <v>45379</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="E19" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>16</v>

</xml_diff>